<commit_message>
Handled the error that is caused if an already opened excel workbook is being updated
</commit_message>
<xml_diff>
--- a/feuillePointage/PointageWorkbook/PointageAnnuel.xlsx
+++ b/feuillePointage/PointageWorkbook/PointageAnnuel.xlsx
@@ -5586,7 +5586,11 @@
         </is>
       </c>
       <c r="O15" s="40" t="n"/>
-      <c r="P15" s="26" t="n"/>
+      <c r="P15" s="26" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="Q15" s="26" t="n"/>
       <c r="R15" s="26" t="n"/>
       <c r="S15" s="26" t="n"/>
@@ -8707,7 +8711,11 @@
         </is>
       </c>
       <c r="O15" s="40" t="n"/>
-      <c r="P15" s="26" t="n"/>
+      <c r="P15" s="26" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
       <c r="Q15" s="26" t="n"/>
       <c r="R15" s="26" t="n"/>
       <c r="S15" s="26" t="n"/>
@@ -11844,7 +11852,11 @@
         </is>
       </c>
       <c r="O15" s="40" t="n"/>
-      <c r="P15" s="26" t="n"/>
+      <c r="P15" s="26" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
       <c r="Q15" s="26" t="n"/>
       <c r="R15" s="26" t="n"/>
       <c r="S15" s="26" t="n"/>
@@ -14977,7 +14989,11 @@
         </is>
       </c>
       <c r="O15" s="40" t="n"/>
-      <c r="P15" s="26" t="n"/>
+      <c r="P15" s="26" t="inlineStr">
+        <is>
+          <t>Cr</t>
+        </is>
+      </c>
       <c r="Q15" s="26" t="n"/>
       <c r="R15" s="26" t="n"/>
       <c r="S15" s="26" t="n"/>

</xml_diff>

<commit_message>
now you can update le pointage of many employees at once
</commit_message>
<xml_diff>
--- a/feuillePointage/PointageWorkbook/PointageAnnuel.xlsx
+++ b/feuillePointage/PointageWorkbook/PointageAnnuel.xlsx
@@ -5591,7 +5591,11 @@
           <t>2</t>
         </is>
       </c>
-      <c r="Q15" s="26" t="n"/>
+      <c r="Q15" s="26" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
       <c r="R15" s="26" t="n"/>
       <c r="S15" s="26" t="n"/>
       <c r="T15" s="26" t="n"/>
@@ -8716,7 +8720,11 @@
           <t>6</t>
         </is>
       </c>
-      <c r="Q15" s="26" t="n"/>
+      <c r="Q15" s="26" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
       <c r="R15" s="26" t="n"/>
       <c r="S15" s="26" t="n"/>
       <c r="T15" s="26" t="n"/>
@@ -14994,7 +15002,11 @@
           <t>Cr</t>
         </is>
       </c>
-      <c r="Q15" s="26" t="n"/>
+      <c r="Q15" s="26" t="inlineStr">
+        <is>
+          <t>T</t>
+        </is>
+      </c>
       <c r="R15" s="26" t="n"/>
       <c r="S15" s="26" t="n"/>
       <c r="T15" s="26" t="n"/>
@@ -18107,7 +18119,11 @@
       <c r="N15" s="26" t="n"/>
       <c r="O15" s="40" t="n"/>
       <c r="P15" s="26" t="n"/>
-      <c r="Q15" s="26" t="n"/>
+      <c r="Q15" s="26" t="inlineStr">
+        <is>
+          <t>Cr</t>
+        </is>
+      </c>
       <c r="R15" s="26" t="n"/>
       <c r="S15" s="26" t="n"/>
       <c r="T15" s="26" t="n"/>

</xml_diff>